<commit_message>
Update app.py and Excel file with latest modifications
</commit_message>
<xml_diff>
--- a/Roadmap_Monitoring_System_2.xlsx
+++ b/Roadmap_Monitoring_System_2.xlsx
@@ -5,22 +5,22 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thiago-ext\Documents\data_science_expert\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thiago-ext\Documents\data_science_expert\progress\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="10500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="10500"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="129">
   <si>
     <t>Objective</t>
   </si>
@@ -788,187 +788,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:I36"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="66" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="35.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="62.109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="79.44140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11" bestFit="1" customWidth="1"/>
+    <col min="1" max="3" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="35.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="39.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="52.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A2">
-        <v>0</v>
-      </c>
-      <c r="B2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D2" t="s">
-        <v>16</v>
-      </c>
-      <c r="E2" t="s">
-        <v>21</v>
-      </c>
-      <c r="F2" t="s">
-        <v>26</v>
-      </c>
-      <c r="G2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A3">
-        <v>1</v>
-      </c>
-      <c r="B3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E3" t="s">
-        <v>22</v>
-      </c>
-      <c r="F3" t="s">
-        <v>26</v>
-      </c>
-      <c r="G3" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A4">
-        <v>2</v>
-      </c>
-      <c r="B4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D4" t="s">
-        <v>18</v>
-      </c>
-      <c r="E4" t="s">
-        <v>23</v>
-      </c>
-      <c r="F4" t="s">
-        <v>26</v>
-      </c>
-      <c r="G4" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A5">
-        <v>3</v>
-      </c>
-      <c r="B5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C5" t="s">
-        <v>14</v>
-      </c>
-      <c r="D5" t="s">
-        <v>19</v>
-      </c>
-      <c r="E5" t="s">
-        <v>24</v>
-      </c>
-      <c r="F5" t="s">
-        <v>26</v>
-      </c>
-      <c r="G5" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A6">
-        <v>4</v>
-      </c>
-      <c r="B6" t="s">
-        <v>10</v>
-      </c>
-      <c r="C6" t="s">
-        <v>15</v>
-      </c>
-      <c r="D6" t="s">
-        <v>20</v>
-      </c>
-      <c r="E6" t="s">
-        <v>25</v>
-      </c>
-      <c r="F6" t="s">
-        <v>26</v>
-      </c>
-      <c r="G6" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A7">
-        <v>5</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I36"/>
-  <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="G23" sqref="G23"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="3" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="35.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.5546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="39.44140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="52.88671875" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>31</v>
       </c>
@@ -997,7 +832,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -1026,7 +861,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>2</v>
       </c>
@@ -1055,7 +890,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <v>4</v>
       </c>
@@ -1084,7 +919,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
         <v>2</v>
       </c>
@@ -1113,7 +948,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
         <v>2</v>
       </c>
@@ -1142,7 +977,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>100</v>
       </c>
@@ -1171,7 +1006,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
         <v>2</v>
       </c>
@@ -1200,7 +1035,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
         <v>2</v>
       </c>
@@ -1225,7 +1060,7 @@
       </c>
       <c r="I9" s="3"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>67</v>
       </c>
@@ -1254,7 +1089,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
         <v>1</v>
       </c>
@@ -1283,7 +1118,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="3">
         <v>2</v>
       </c>
@@ -1312,7 +1147,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="3">
         <v>2</v>
       </c>
@@ -1341,7 +1176,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
         <v>67</v>
       </c>
@@ -1370,7 +1205,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>67</v>
       </c>
@@ -1399,7 +1234,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="3">
         <v>2</v>
       </c>
@@ -1424,7 +1259,7 @@
       </c>
       <c r="I16" s="3"/>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="3">
         <v>4</v>
       </c>
@@ -1453,7 +1288,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="3">
         <v>4</v>
       </c>
@@ -1482,7 +1317,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="3">
         <v>2</v>
       </c>
@@ -1507,7 +1342,7 @@
       </c>
       <c r="I19" s="3"/>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="3">
         <v>2</v>
       </c>
@@ -1536,7 +1371,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="3">
         <v>2</v>
       </c>
@@ -1561,7 +1396,7 @@
       </c>
       <c r="I21" s="3"/>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="3">
         <v>1</v>
       </c>
@@ -1590,7 +1425,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="3">
         <v>2</v>
       </c>
@@ -1619,7 +1454,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="3">
         <v>2</v>
       </c>
@@ -1648,7 +1483,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="3">
         <v>2</v>
       </c>
@@ -1675,7 +1510,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="3">
         <v>2</v>
       </c>
@@ -1700,7 +1535,7 @@
       </c>
       <c r="I26" s="3"/>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="3">
         <v>3</v>
       </c>
@@ -1725,9 +1560,11 @@
       <c r="H27" s="3">
         <v>36</v>
       </c>
-      <c r="I27" s="3"/>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="I27" s="3" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="3">
         <v>4</v>
       </c>
@@ -1754,7 +1591,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="3">
         <v>4</v>
       </c>
@@ -1783,7 +1620,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" s="3">
         <v>4</v>
       </c>
@@ -1812,7 +1649,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" s="3">
         <v>4</v>
       </c>
@@ -1841,7 +1678,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" s="3">
         <v>2</v>
       </c>
@@ -1870,7 +1707,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" s="3">
         <v>2</v>
       </c>
@@ -1899,7 +1736,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" s="3">
         <v>1</v>
       </c>
@@ -1928,7 +1765,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" s="7">
         <v>1</v>
       </c>
@@ -1957,7 +1794,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" s="7">
         <v>1</v>
       </c>
@@ -1989,4 +1826,169 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C28" sqref="C28"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="66" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="35.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="62.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="79.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F2" t="s">
+        <v>26</v>
+      </c>
+      <c r="G2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F3" t="s">
+        <v>26</v>
+      </c>
+      <c r="G3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" t="s">
+        <v>18</v>
+      </c>
+      <c r="E4" t="s">
+        <v>23</v>
+      </c>
+      <c r="F4" t="s">
+        <v>26</v>
+      </c>
+      <c r="G4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" t="s">
+        <v>19</v>
+      </c>
+      <c r="E5" t="s">
+        <v>24</v>
+      </c>
+      <c r="F5" t="s">
+        <v>26</v>
+      </c>
+      <c r="G5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6" t="s">
+        <v>20</v>
+      </c>
+      <c r="E6" t="s">
+        <v>25</v>
+      </c>
+      <c r="F6" t="s">
+        <v>26</v>
+      </c>
+      <c r="G6" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Update Excel file with latest data
</commit_message>
<xml_diff>
--- a/Roadmap_Monitoring_System_2.xlsx
+++ b/Roadmap_Monitoring_System_2.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="130">
   <si>
     <t>Objective</t>
   </si>
@@ -190,9 +190,6 @@
     <t>LISER</t>
   </si>
   <si>
-    <t>21/07/205</t>
-  </si>
-  <si>
     <t>Maxence De Valière</t>
   </si>
   <si>
@@ -241,9 +238,6 @@
     <t>UPSKILL</t>
   </si>
   <si>
-    <t>01/01/205</t>
-  </si>
-  <si>
     <t>WKP preparation and revision</t>
   </si>
   <si>
@@ -407,6 +401,15 @@
   </si>
   <si>
     <t>Project</t>
+  </si>
+  <si>
+    <t>Auditing VAT</t>
+  </si>
+  <si>
+    <t>prepare docs</t>
+  </si>
+  <si>
+    <t>Correction paper</t>
   </si>
 </sst>
 </file>
@@ -788,10 +791,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I36"/>
+  <dimension ref="A1:I39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F27" sqref="F27"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="C39" sqref="C39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -907,10 +910,10 @@
         <v>55</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="H4" s="3">
         <v>20</v>
@@ -936,10 +939,10 @@
         <v>46</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="H5" s="3">
         <v>25</v>
@@ -965,10 +968,10 @@
         <v>46</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="H6" s="3">
         <v>80</v>
@@ -979,7 +982,7 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B7" s="4">
         <v>45839</v>
@@ -988,16 +991,16 @@
         <v>45925</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="H7" s="3">
         <v>16</v>
@@ -1044,16 +1047,16 @@
       </c>
       <c r="C9" s="3"/>
       <c r="D9" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="G9" s="3" t="s">
         <v>78</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="F9" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="G9" s="3" t="s">
-        <v>80</v>
       </c>
       <c r="H9" s="3">
         <v>6</v>
@@ -1062,7 +1065,7 @@
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B10" s="4">
         <v>45848</v>
@@ -1071,16 +1074,16 @@
         <v>45998</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="H10" s="3">
         <v>15</v>
@@ -1100,16 +1103,16 @@
         <v>45856</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="E11" s="3" t="s">
         <v>46</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="H11" s="3">
         <v>2</v>
@@ -1129,16 +1132,16 @@
         <v>45916</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="E12" s="3" t="s">
         <v>46</v>
       </c>
       <c r="F12" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="G12" s="3" t="s">
         <v>94</v>
-      </c>
-      <c r="G12" s="3" t="s">
-        <v>96</v>
       </c>
       <c r="H12" s="3">
         <v>8</v>
@@ -1178,7 +1181,7 @@
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B14" s="4">
         <v>45908</v>
@@ -1187,16 +1190,16 @@
         <v>45919</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E14" s="3" t="s">
         <v>46</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="H14" s="3">
         <v>80</v>
@@ -1207,7 +1210,7 @@
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B15" s="4">
         <v>45911</v>
@@ -1216,16 +1219,16 @@
         <v>45911</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E15" s="3" t="s">
         <v>46</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="G15" s="3" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="H15" s="3">
         <v>4</v>
@@ -1243,16 +1246,16 @@
       </c>
       <c r="C16" s="3"/>
       <c r="D16" s="3" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="E16" s="3" t="s">
         <v>55</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="G16" s="3" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="H16" s="3">
         <v>1</v>
@@ -1270,16 +1273,16 @@
         <v>46000</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E17" s="3" t="s">
         <v>55</v>
       </c>
       <c r="F17" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="G17" s="3" t="s">
         <v>69</v>
-      </c>
-      <c r="G17" s="3" t="s">
-        <v>70</v>
       </c>
       <c r="H17" s="3">
         <v>4</v>
@@ -1308,7 +1311,7 @@
         <v>42</v>
       </c>
       <c r="G18" s="3" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="H18" s="3">
         <v>3</v>
@@ -1321,8 +1324,8 @@
       <c r="A19" s="3">
         <v>2</v>
       </c>
-      <c r="B19" s="3" t="s">
-        <v>73</v>
+      <c r="B19" s="4">
+        <v>45658</v>
       </c>
       <c r="C19" s="3"/>
       <c r="D19" s="3" t="s">
@@ -1332,10 +1335,10 @@
         <v>37</v>
       </c>
       <c r="F19" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="G19" s="3" t="s">
         <v>72</v>
-      </c>
-      <c r="G19" s="3" t="s">
-        <v>74</v>
       </c>
       <c r="H19" s="3">
         <v>8</v>
@@ -1346,23 +1349,23 @@
       <c r="A20" s="3">
         <v>2</v>
       </c>
-      <c r="B20" s="3" t="s">
-        <v>56</v>
+      <c r="B20" s="4">
+        <v>45859</v>
       </c>
       <c r="C20" s="4">
         <v>45869</v>
       </c>
       <c r="D20" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="E20" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="E20" s="3" t="s">
+      <c r="F20" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="F20" s="3" t="s">
+      <c r="G20" s="3" t="s">
         <v>59</v>
-      </c>
-      <c r="G20" s="3" t="s">
-        <v>60</v>
       </c>
       <c r="H20" s="3">
         <v>10</v>
@@ -1376,20 +1379,20 @@
         <v>2</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C21" s="3"/>
       <c r="D21" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E21" s="3" t="s">
         <v>37</v>
       </c>
       <c r="F21" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="G21" s="3" t="s">
         <v>63</v>
-      </c>
-      <c r="G21" s="3" t="s">
-        <v>64</v>
       </c>
       <c r="H21" s="3">
         <v>5</v>
@@ -1401,13 +1404,13 @@
         <v>1</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="E22" s="3" t="s">
         <v>37</v>
@@ -1416,7 +1419,7 @@
         <v>38</v>
       </c>
       <c r="G22" s="3" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="H22" s="3">
         <v>0.5</v>
@@ -1430,22 +1433,22 @@
         <v>2</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C23" s="4">
         <v>45986</v>
       </c>
       <c r="D23" s="6" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="E23" s="3" t="s">
         <v>37</v>
       </c>
       <c r="F23" s="3" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="G23" s="3" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="H23" s="3">
         <v>12</v>
@@ -1465,16 +1468,16 @@
         <v>45912</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="F24" s="3" t="s">
         <v>38</v>
       </c>
       <c r="G24" s="3" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="H24" s="3">
         <v>8</v>
@@ -1492,16 +1495,16 @@
       </c>
       <c r="C25" s="4"/>
       <c r="D25" s="3" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="E25" s="3" t="s">
         <v>46</v>
       </c>
       <c r="F25" s="3" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="G25" s="3" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="H25" s="3">
         <v>4</v>
@@ -1519,16 +1522,16 @@
       </c>
       <c r="C26" s="3"/>
       <c r="D26" s="3" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="F26" s="3" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="G26" s="3" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="H26" s="3">
         <v>4</v>
@@ -1546,16 +1549,16 @@
         <v>45996</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="F27" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="G27" s="3" t="s">
         <v>111</v>
-      </c>
-      <c r="G27" s="3" t="s">
-        <v>113</v>
       </c>
       <c r="H27" s="3">
         <v>36</v>
@@ -1579,10 +1582,10 @@
         <v>46</v>
       </c>
       <c r="F28" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="G28" s="3" t="s">
         <v>112</v>
-      </c>
-      <c r="G28" s="3" t="s">
-        <v>114</v>
       </c>
       <c r="H28" s="3">
         <v>4</v>
@@ -1602,16 +1605,16 @@
         <v>45951</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="F29" s="3" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="G29" s="3" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="H29" s="3">
         <v>4</v>
@@ -1631,16 +1634,16 @@
         <v>45974</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="E30" s="3" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="F30" s="3" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="G30" s="3" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="H30" s="3">
         <v>4</v>
@@ -1666,10 +1669,10 @@
         <v>37</v>
       </c>
       <c r="F31" s="3" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="G31" s="3" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="H31" s="3">
         <v>16</v>
@@ -1686,7 +1689,7 @@
         <v>45973</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="D32" s="3" t="s">
         <v>40</v>
@@ -1695,10 +1698,10 @@
         <v>37</v>
       </c>
       <c r="F32" s="3" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="G32" s="3" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="H32" s="3">
         <v>2</v>
@@ -1724,10 +1727,10 @@
         <v>46</v>
       </c>
       <c r="F33" s="3" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="G33" s="3" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="H33" s="3">
         <v>6</v>
@@ -1747,16 +1750,16 @@
         <v>45995</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="E34" s="3" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="F34" s="3" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="G34" s="3" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="H34" s="3">
         <v>8</v>
@@ -1776,16 +1779,16 @@
         <v>46031</v>
       </c>
       <c r="D35" s="7" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="E35" s="7" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="F35" s="7" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="G35" s="7" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="H35" s="7">
         <v>40</v>
@@ -1803,21 +1806,90 @@
       </c>
       <c r="C36" s="2"/>
       <c r="D36" s="7" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="E36" s="7" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="F36" s="7" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="G36" s="7" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="H36" s="7">
         <v>24</v>
       </c>
       <c r="I36" s="7"/>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A37" s="3">
+        <v>0</v>
+      </c>
+      <c r="B37" s="2">
+        <v>46041</v>
+      </c>
+      <c r="D37" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="E37" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="F37" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="G37" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="H37" s="3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A38" s="3">
+        <v>3</v>
+      </c>
+      <c r="B38" s="2">
+        <v>46042</v>
+      </c>
+      <c r="D38" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="E38" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="F38" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="G38" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="H38" s="3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A39" s="3">
+        <v>4</v>
+      </c>
+      <c r="B39" s="2">
+        <v>46043</v>
+      </c>
+      <c r="D39" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="E39" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="F39" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="G39" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="H39" s="3">
+        <v>4</v>
+      </c>
     </row>
   </sheetData>
   <sortState ref="A2:I22">

</xml_diff>

<commit_message>
Update Excel file with additional changes
</commit_message>
<xml_diff>
--- a/Roadmap_Monitoring_System_2.xlsx
+++ b/Roadmap_Monitoring_System_2.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="132">
   <si>
     <t>Objective</t>
   </si>
@@ -410,6 +410,12 @@
   </si>
   <si>
     <t>Correction paper</t>
+  </si>
+  <si>
+    <t>Monitoring System</t>
+  </si>
+  <si>
+    <t>app</t>
   </si>
 </sst>
 </file>
@@ -474,7 +480,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -487,6 +493,7 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -791,10 +798,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I39"/>
+  <dimension ref="A1:I41"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="C39" sqref="C39"/>
+      <selection activeCell="F39" sqref="F39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1115,7 +1122,7 @@
         <v>75</v>
       </c>
       <c r="H11" s="3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I11" s="3" t="s">
         <v>44</v>
@@ -1798,97 +1805,148 @@
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A36" s="7">
-        <v>1</v>
-      </c>
-      <c r="B36" s="2">
-        <v>46034</v>
-      </c>
-      <c r="C36" s="2"/>
+      <c r="A36" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="B36" s="8">
+        <v>45672</v>
+      </c>
+      <c r="C36" s="8"/>
       <c r="D36" s="7" t="s">
-        <v>76</v>
+        <v>67</v>
       </c>
       <c r="E36" s="7" t="s">
         <v>77</v>
       </c>
       <c r="F36" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="G36" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="H36" s="7">
+        <v>2</v>
+      </c>
+      <c r="I36" s="3"/>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A37" s="7">
+        <v>1</v>
+      </c>
+      <c r="B37" s="8">
+        <v>46034</v>
+      </c>
+      <c r="C37" s="8"/>
+      <c r="D37" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="E37" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="F37" s="7" t="s">
         <v>125</v>
       </c>
-      <c r="G36" s="7" t="s">
+      <c r="G37" s="7" t="s">
         <v>126</v>
       </c>
-      <c r="H36" s="7">
+      <c r="H37" s="7">
         <v>24</v>
       </c>
-      <c r="I36" s="7"/>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A37" s="3">
+      <c r="I37" s="7"/>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A38" s="7">
         <v>0</v>
       </c>
-      <c r="B37" s="2">
+      <c r="B38" s="8">
         <v>46041</v>
       </c>
-      <c r="D37" s="3" t="s">
+      <c r="C38" s="7"/>
+      <c r="D38" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="E37" s="3" t="s">
+      <c r="E38" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="F37" s="3" t="s">
+      <c r="F38" s="7" t="s">
         <v>127</v>
       </c>
-      <c r="G37" s="3" t="s">
+      <c r="G38" s="7" t="s">
         <v>128</v>
       </c>
-      <c r="H37" s="3">
+      <c r="H38" s="7">
         <v>8</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A38" s="3">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A39" s="7">
         <v>3</v>
       </c>
-      <c r="B38" s="2">
+      <c r="B39" s="8">
         <v>46042</v>
       </c>
-      <c r="D38" s="3" t="s">
+      <c r="C39" s="7"/>
+      <c r="D39" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="E38" s="3" t="s">
+      <c r="E39" s="7" t="s">
         <v>77</v>
       </c>
-      <c r="F38" s="3" t="s">
+      <c r="F39" s="7" t="s">
         <v>86</v>
       </c>
-      <c r="G38" s="3" t="s">
+      <c r="G39" s="7" t="s">
         <v>85</v>
       </c>
-      <c r="H38" s="3">
+      <c r="H39" s="7">
         <v>8</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A39" s="3">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A40" s="7">
         <v>4</v>
       </c>
-      <c r="B39" s="2">
+      <c r="B40" s="8">
         <v>46043</v>
       </c>
-      <c r="D39" s="3" t="s">
+      <c r="C40" s="7"/>
+      <c r="D40" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="E39" s="3" t="s">
+      <c r="E40" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="F39" s="3" t="s">
+      <c r="F40" s="7" t="s">
         <v>80</v>
       </c>
-      <c r="G39" s="3" t="s">
+      <c r="G40" s="7" t="s">
         <v>129</v>
       </c>
-      <c r="H39" s="3">
+      <c r="H40" s="7">
         <v>4</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A41" s="7">
+        <v>4</v>
+      </c>
+      <c r="B41" s="8">
+        <v>46038</v>
+      </c>
+      <c r="D41" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="E41" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="F41" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="G41" s="7" t="s">
+        <v>131</v>
+      </c>
+      <c r="H41" s="7">
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update Excel file with latest modifications
</commit_message>
<xml_diff>
--- a/Roadmap_Monitoring_System_2.xlsx
+++ b/Roadmap_Monitoring_System_2.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="135">
   <si>
     <t>Objective</t>
   </si>
@@ -416,6 +416,15 @@
   </si>
   <si>
     <t>app</t>
+  </si>
+  <si>
+    <t>2026 plan</t>
+  </si>
+  <si>
+    <t>prepare the options for AI strategy</t>
+  </si>
+  <si>
+    <t>22/01/20296</t>
   </si>
 </sst>
 </file>
@@ -798,10 +807,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I41"/>
+  <dimension ref="A1:I43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="F39" sqref="F39"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="F46" sqref="F46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1388,7 +1397,9 @@
       <c r="B21" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="C21" s="3"/>
+      <c r="C21" s="4">
+        <v>46387</v>
+      </c>
       <c r="D21" s="3" t="s">
         <v>61</v>
       </c>
@@ -1404,7 +1415,9 @@
       <c r="H21" s="3">
         <v>5</v>
       </c>
-      <c r="I21" s="3"/>
+      <c r="I21" s="3" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="3">
@@ -1948,6 +1961,60 @@
       <c r="H41" s="7">
         <v>8</v>
       </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A42" s="7">
+        <v>2</v>
+      </c>
+      <c r="B42" s="2">
+        <v>46044</v>
+      </c>
+      <c r="C42" s="2">
+        <v>46045</v>
+      </c>
+      <c r="D42" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="E42" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="F42" s="7" t="s">
+        <v>132</v>
+      </c>
+      <c r="G42" s="7" t="s">
+        <v>133</v>
+      </c>
+      <c r="H42" s="7">
+        <v>8</v>
+      </c>
+      <c r="I42" s="7" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A43" s="7">
+        <v>2</v>
+      </c>
+      <c r="B43" s="7" t="s">
+        <v>134</v>
+      </c>
+      <c r="C43" s="8"/>
+      <c r="D43" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="E43" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="F43" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="G43" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="H43" s="7">
+        <v>8</v>
+      </c>
+      <c r="I43" s="7"/>
     </row>
   </sheetData>
   <sortState ref="A2:I22">

</xml_diff>